<commit_message>
Add web scraping and modify client
</commit_message>
<xml_diff>
--- a/flask-server/courses.xlsx
+++ b/flask-server/courses.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>ID</t>
   </si>
@@ -28,61 +28,67 @@
     <t>Type</t>
   </si>
   <si>
-    <t>OOP</t>
+    <t>Semester</t>
+  </si>
+  <si>
+    <t>Package</t>
+  </si>
+  <si>
+    <t>Object oriented programming</t>
   </si>
   <si>
     <t>Compulsory</t>
   </si>
   <si>
-    <t>DSA</t>
-  </si>
-  <si>
-    <t>DBMS</t>
-  </si>
-  <si>
-    <t>ASC</t>
-  </si>
-  <si>
-    <t>FP</t>
-  </si>
-  <si>
-    <t>AI</t>
-  </si>
-  <si>
-    <t>FLCD</t>
-  </si>
-  <si>
-    <t>OS</t>
-  </si>
-  <si>
-    <t>MOBILE</t>
-  </si>
-  <si>
-    <t>NET</t>
-  </si>
-  <si>
-    <t>AT</t>
+    <t>Data structures and algorithms</t>
+  </si>
+  <si>
+    <t>Database management systems</t>
+  </si>
+  <si>
+    <t>Computer systems architecture</t>
+  </si>
+  <si>
+    <t>Functional and logic programming</t>
+  </si>
+  <si>
+    <t>Artificial intelligence</t>
+  </si>
+  <si>
+    <t>Formal languages and compiler design</t>
+  </si>
+  <si>
+    <t>Operating systems</t>
+  </si>
+  <si>
+    <t>Mobile application programming</t>
+  </si>
+  <si>
+    <t>Computer networks</t>
+  </si>
+  <si>
+    <t>Android things</t>
   </si>
   <si>
     <t>Optional</t>
   </si>
   <si>
-    <t>IOT</t>
-  </si>
-  <si>
-    <t>SNA</t>
-  </si>
-  <si>
-    <t>DP</t>
-  </si>
-  <si>
-    <t>ACD</t>
-  </si>
-  <si>
-    <t>CH</t>
-  </si>
-  <si>
-    <t>EI</t>
+    <t>Computer science investigations -an iot perspective</t>
+  </si>
+  <si>
+    <t>Network and system administration</t>
+  </si>
+  <si>
+    <t>Design patterns</t>
+  </si>
+  <si>
+    <t>Advanced compiler design</t>
+  </si>
+  <si>
+    <t>History of computer science</t>
+  </si>
+  <si>
+    <t>Academic ethics and integrity (in computer science)</t>
   </si>
 </sst>
 </file>
@@ -463,16 +469,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="42.14785714285715" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -488,17 +496,29 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
@@ -506,23 +526,35 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="22.5">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="E4" s="3">
+        <v>3</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
@@ -530,35 +562,53 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="23.25">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="23.25">
+        <v>7</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="E7" s="3">
+        <v>4</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
@@ -566,11 +616,17 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="3">
         <v>5</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
@@ -578,11 +634,17 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="E9" s="3">
+        <v>2</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
@@ -590,23 +652,35 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="21.75">
+        <v>7</v>
+      </c>
+      <c r="E10" s="3">
+        <v>4</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="3">
         <v>5</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
@@ -614,23 +688,35 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18">
+        <v>18</v>
+      </c>
+      <c r="E12" s="3">
+        <v>5</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="E13" s="3">
+        <v>5</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
@@ -638,23 +724,35 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="22.5">
+        <v>18</v>
+      </c>
+      <c r="E14" s="3">
+        <v>5</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="E15" s="3">
+        <v>5</v>
+      </c>
+      <c r="F15" s="3">
+        <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
@@ -662,23 +760,35 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="23.25">
+        <v>18</v>
+      </c>
+      <c r="E16" s="3">
+        <v>5</v>
+      </c>
+      <c r="F16" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="E17" s="3">
+        <v>6</v>
+      </c>
+      <c r="F17" s="3">
+        <v>3</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
@@ -686,11 +796,17 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="E18" s="3">
+        <v>6</v>
+      </c>
+      <c r="F18" s="3">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>